<commit_message>
Script de base de datos en carpeta SCRIPT DATA de la carpeta database, la soluciòn sigue siendo WEB DINAMICO 2, ya se encuentran con los cambios y nuevos archvivos de los cambios
</commit_message>
<xml_diff>
--- a/back-end/Web Dinamico 2/MRVMinem/Documentos/1.1 Plantilla_Etiquetado_de_eficiencia_ Aire acondicionado.xlsx
+++ b/back-end/Web Dinamico 2/MRVMinem/Documentos/1.1 Plantilla_Etiquetado_de_eficiencia_ Aire acondicionado.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\Versiòn plantillas\Versión borrado de meses y fechas SOLO SE DEJO AÑOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\Versión borrado de meses y fechas SOLO SE DEJO AÑOS _V2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39820C21-8B25-409E-AF9A-EC89B890BB54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC62BAD7-D369-4AA5-A305-8670E752AF6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{0FF7017A-1C1F-4F31-834A-BE5FD5CEB108}"/>
+    <workbookView xWindow="-15480" yWindow="-120" windowWidth="15600" windowHeight="11310" xr2:uid="{0FF7017A-1C1F-4F31-834A-BE5FD5CEB108}"/>
   </bookViews>
   <sheets>
     <sheet name="Aire Acondicionado" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
   <si>
     <t>Año</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Etiqueta BAU</t>
   </si>
   <si>
-    <t>Etiqueta Iniciativa</t>
-  </si>
-  <si>
     <t>Cantidad</t>
   </si>
   <si>
@@ -70,12 +67,6 @@
   </si>
   <si>
     <t>Mini Split 9000 - 12000 BTU</t>
-  </si>
-  <si>
-    <t>Mini Split 12000 - 1800 BTU</t>
-  </si>
-  <si>
-    <t>Mini Split 18000 - 2400 BTU</t>
   </si>
   <si>
     <t>_</t>
@@ -150,12 +141,6 @@
     <t>24000 - 30000 BTU</t>
   </si>
   <si>
-    <t>Etiqueta del equipo anterior o reemplazado. Seleccione de lista desplegable.</t>
-  </si>
-  <si>
-    <t>Etiqueta del equipo nuevo. Seleccione de lista desplegable.</t>
-  </si>
-  <si>
     <t>Número de unidades de este equipo. Inserte su dato.</t>
   </si>
   <si>
@@ -166,6 +151,24 @@
   </si>
   <si>
     <t>Registrar sus datos según el ejemplo brindado. Borre estos datos y complete los suyos.</t>
+  </si>
+  <si>
+    <t>Mini Split 12000 - 18000 BTU</t>
+  </si>
+  <si>
+    <t>Mini Split 18000 - 24000 BTU</t>
+  </si>
+  <si>
+    <t>Etiqueta de EE BAU</t>
+  </si>
+  <si>
+    <t>Etiqueta de EE Acción</t>
+  </si>
+  <si>
+    <t>Etiqueta de EE del equipo anterior o reemplazado. Seleccione de la lista desplegable.</t>
+  </si>
+  <si>
+    <t>Etiqueta de EE del equipo nuevo. Seleccione de la lista desplegable.</t>
   </si>
 </sst>
 </file>
@@ -664,10 +667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2029263-33DE-46C6-ADE8-A69CDB86AC1C}">
-  <dimension ref="A1:I311"/>
+  <dimension ref="A1:H311"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,21 +699,21 @@
         <v>1</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="13" t="s">
         <v>4</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
@@ -722,22 +725,22 @@
     </row>
     <row r="3" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="11" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="11" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F3" s="12"/>
       <c r="G3" s="11" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -746,24 +749,24 @@
       </c>
       <c r="B4" s="17">
         <f t="shared" ref="B4:B67" si="0">VLOOKUP(C4,Tabla_Capacidad,2,)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D4" s="17">
         <f t="shared" ref="D4:D67" si="1">VLOOKUP(E4,Tabla_BAU,2,)</f>
         <v>5</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F4" s="17">
         <f t="shared" ref="F4:F67" si="2">VLOOKUP(G4,Tabla_Iniciativa,2,)</f>
         <v>1</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H4" s="18">
         <v>100000</v>
@@ -6603,7 +6606,7 @@
       <c r="H311" s="15"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="596P/ajDNkLEgtdMrrPEIZdgk6Lly3QzrZrrvg9rwRopgRocP6V+vHpUC1kvjL17hhEOmfX+aiDUni/afaSBdA==" saltValue="T8PGgoFwLXJoDW0pQ0sa/w==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="1">
     <mergeCell ref="A2:H2"/>
   </mergeCells>
@@ -6639,13 +6642,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B5CEF2D-D2B2-49FA-B326-3BFB82F55E48}">
   <dimension ref="A4:M62"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1"/>
     <col min="6" max="6" width="33.7109375" customWidth="1"/>
     <col min="9" max="9" width="19.28515625" customWidth="1"/>
   </cols>
@@ -6670,28 +6673,28 @@
         <v>2012</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -6699,25 +6702,25 @@
         <v>2013</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" s="5">
         <v>1</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G8" s="5">
         <v>1</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="J8" s="5">
         <v>1</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="M8" s="5">
         <v>1</v>
@@ -6728,25 +6731,25 @@
         <v>2014</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="D9" s="5">
         <v>2</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G9" s="5">
         <v>2</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J9" s="5">
         <v>2</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="M9" s="5">
         <v>2</v>
@@ -6757,25 +6760,25 @@
         <v>2015</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="D10" s="5">
         <v>3</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G10" s="5">
         <v>3</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J10" s="5">
         <v>3</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="M10" s="5">
         <v>3</v>
@@ -6786,25 +6789,25 @@
         <v>2016</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D11" s="5">
         <v>4</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G11" s="5">
         <v>4</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="J11" s="5">
         <v>4</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="M11" s="5">
         <v>4</v>
@@ -6815,25 +6818,25 @@
         <v>2017</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D12" s="5">
         <v>5</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G12" s="5">
         <v>5</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J12" s="5">
         <v>5</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="M12" s="5">
         <v>5</v>
@@ -6844,19 +6847,19 @@
         <v>2018</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G13" s="5">
         <v>6</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="J13" s="5">
         <v>6</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="M13" s="5">
         <v>6</v>
@@ -6867,19 +6870,19 @@
         <v>2019</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G14" s="5">
         <v>7</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J14" s="5">
         <v>7</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="M14" s="5">
         <v>7</v>
@@ -6890,7 +6893,7 @@
         <v>2020</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="M15" s="5">
         <v>8</v>
@@ -6901,7 +6904,7 @@
         <v>2021</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="M16" s="5">
         <v>9</v>
@@ -6912,7 +6915,7 @@
         <v>2022</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="M17" s="5">
         <v>10</v>
@@ -6923,7 +6926,7 @@
         <v>2023</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="M18" s="5">
         <v>11</v>
@@ -6934,7 +6937,7 @@
         <v>2024</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="M19" s="5">
         <v>12</v>
@@ -6975,7 +6978,7 @@
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>